<commit_message>
Cambios para poder hacer pull
</commit_message>
<xml_diff>
--- a/ArrendaSys/TempFolder/Excel02-11-2021.xlsx
+++ b/ArrendaSys/TempFolder/Excel02-11-2021.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>1☆</t>
   </si>
@@ -30,6 +30,12 @@
   </si>
   <si>
     <t>Cumplimiento de pago</t>
+  </si>
+  <si>
+    <t>Cuidado del Inmueble</t>
+  </si>
+  <si>
+    <t>Responsabilidad General</t>
   </si>
 </sst>
 </file>
@@ -141,12 +147,12 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!A2:A2</c:f>
+              <c:f>Sheet1!A2:A4</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!B2</c:f>
+              <c:f>Sheet1!B2:B4</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -165,12 +171,12 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!A2:A2</c:f>
+              <c:f>Sheet1!A2:A4</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!C2</c:f>
+              <c:f>Sheet1!C2:C4</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -189,12 +195,12 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!A2:A2</c:f>
+              <c:f>Sheet1!A2:A4</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!D2</c:f>
+              <c:f>Sheet1!D2:D4</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -213,12 +219,12 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!A2:A2</c:f>
+              <c:f>Sheet1!A2:A4</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!E2</c:f>
+              <c:f>Sheet1!E2:E4</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -237,12 +243,12 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!A2:A2</c:f>
+              <c:f>Sheet1!A2:A4</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!F2</c:f>
+              <c:f>Sheet1!F2:F4</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -344,7 +350,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -370,13 +376,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.3368944440569" customWidth="1"/>
+    <col min="1" max="1" width="23.1160060337612" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
@@ -405,20 +411,33 @@
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0">
+      <c r="C2" s="0">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0">
         <v>2</v>
       </c>
-      <c r="C2" s="0">
-        <v>2</v>
-      </c>
-      <c r="D2" s="0">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0">
-        <v>1</v>
-      </c>
-      <c r="F2" s="0">
-        <v>2</v>
+      <c r="F4" s="0">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>